<commit_message>
Halozatok I. jegyzetek, projectek
</commit_message>
<xml_diff>
--- a/ProgTechGy/y2xwhj_pt_beadando/Funkciok_listaja_2023.xlsx
+++ b/ProgTechGy/y2xwhj_pt_beadando/Funkciok_listaja_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Main\tanulas\ekke\EKKE-4\ProgTechGy\y2xwhj_pt_beadando\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DD7030-8F6A-4AC6-B24C-95F1ADBCAF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C3F22D-F6DB-48E2-8801-697ABBF0DE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1542,7 +1542,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -1635,7 +1635,7 @@
         <v>0.5</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="39.950000000000003" customHeight="1">
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B22" s="9">
         <f>SUMIF(C3:C21,Munka1!A2,B3:B21)</f>
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="C22" s="10"/>
     </row>

</xml_diff>